<commit_message>
working on the experiment
</commit_message>
<xml_diff>
--- a/03_Materials/finalstimuli_list.xlsx
+++ b/03_Materials/finalstimuli_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/SPAML/SPAML-PSA/03_Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2 projects/SPAML/SPAML-PSA/03_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB933A3-7C90-674D-8A00-CEF1908CFAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A6B7CD-C808-FA4D-B71C-EDDDD39D3EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="500" windowWidth="21600" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="760" windowWidth="21600" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="finalstimuli" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="2998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="3000">
   <si>
     <t>en_cue</t>
   </si>
@@ -9028,6 +9028,12 @@
   </si>
   <si>
     <t>aidshiv</t>
+  </si>
+  <si>
+    <t>ling</t>
+  </si>
+  <si>
+    <t>ming</t>
   </si>
 </sst>
 </file>
@@ -10239,8 +10245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1911"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A526" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A538" sqref="A538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16342,7 +16348,10 @@
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A537" s="2" t="s">
-        <v>1679</v>
+        <v>2999</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>2998</v>
       </c>
       <c r="C537" t="s">
         <v>1679</v>

</xml_diff>